<commit_message>
making video page header
</commit_message>
<xml_diff>
--- a/workflow/readme_excel.xlsx
+++ b/workflow/readme_excel.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stanley/Downloads/other/coding/cabletv/cable_website_nextjs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stanley/Downloads/other/coding/cabletv/cable_website_nextjs/workflow/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F233B3A-7AD4-1643-A594-BA79082E3E3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B842CE91-B4F7-814C-9525-5ACBADB4B39C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="32380" windowHeight="20500" xr2:uid="{3A02345B-B633-7141-95EC-F38D4509DA38}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$E$11</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$F$34</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="40">
   <si>
     <t>No</t>
   </si>
@@ -66,10 +66,6 @@
     <t>Video page</t>
   </si>
   <si>
-    <t>videojs is functional
-preroll-ads is not finished</t>
-  </si>
-  <si>
     <t>using ent api</t>
   </si>
   <si>
@@ -82,26 +78,92 @@
     <t>login</t>
   </si>
   <si>
-    <t>comment section</t>
-  </si>
-  <si>
-    <t>live</t>
-  </si>
-  <si>
-    <t>80% done, working on displaying video list</t>
-  </si>
-  <si>
-    <t>Home page responsive</t>
-  </si>
-  <si>
     <t>navbar</t>
+  </si>
+  <si>
+    <t>Sub tasks</t>
+  </si>
+  <si>
+    <t>responseive design</t>
+  </si>
+  <si>
+    <t>header</t>
+  </si>
+  <si>
+    <t>full menu</t>
+  </si>
+  <si>
+    <t>mobile menu</t>
+  </si>
+  <si>
+    <t>search box</t>
+  </si>
+  <si>
+    <t>footer</t>
+  </si>
+  <si>
+    <t>video page header</t>
+  </si>
+  <si>
+    <t>video page footer</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>redirect to video page</t>
+  </si>
+  <si>
+    <t>emoji comment section</t>
+  </si>
+  <si>
+    <t>text comment section</t>
+  </si>
+  <si>
+    <t>video player</t>
+  </si>
+  <si>
+    <t>autoplay is ok, ima is not done</t>
+  </si>
+  <si>
+    <t>scroll down change content</t>
+  </si>
+  <si>
+    <t>moblle menu</t>
+  </si>
+  <si>
+    <t>working now</t>
+  </si>
+  <si>
+    <t>search page</t>
+  </si>
+  <si>
+    <t>tag list page</t>
+  </si>
+  <si>
+    <t>done (redirect to pages)</t>
+  </si>
+  <si>
+    <t>live page</t>
+  </si>
+  <si>
+    <t>emoji box</t>
+  </si>
+  <si>
+    <t>word size</t>
+  </si>
+  <si>
+    <t>share box</t>
+  </si>
+  <si>
+    <t>facebook share</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -115,6 +177,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -124,7 +192,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -223,7 +291,7 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
+      <left style="thin">
         <color indexed="64"/>
       </left>
       <right style="thin">
@@ -241,7 +309,7 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
+      <right style="medium">
         <color indexed="64"/>
       </right>
       <top style="thin">
@@ -253,21 +321,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -304,13 +357,109 @@
         <color indexed="64"/>
       </top>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -327,26 +476,23 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -358,6 +504,51 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -677,180 +868,552 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="108" zoomScaleNormal="100" zoomScaleSheetLayoutView="108" workbookViewId="0">
+      <selection activeCell="G47" sqref="G47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.83203125" style="1"/>
-    <col min="2" max="2" width="17" style="1" customWidth="1"/>
-    <col min="3" max="4" width="29.83203125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="11.83203125" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="10.83203125" style="1"/>
+    <col min="2" max="2" width="15.83203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="17" style="1" customWidth="1"/>
+    <col min="4" max="5" width="29.83203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="11.83203125" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="15"/>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="14"/>
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="14"/>
-      <c r="B2" s="16"/>
-      <c r="C2" s="2" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="13"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="5"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="6">
+      <c r="F2" s="5"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="19">
         <v>1</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="16" t="s">
         <v>6</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="20"/>
+      <c r="B4" s="17"/>
+      <c r="C4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" s="5"/>
+    </row>
+    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.2">
+      <c r="A5" s="21"/>
+      <c r="B5" s="18"/>
+      <c r="C5" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="5"/>
+    </row>
+    <row r="6" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="A6" s="19">
+        <v>2</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="A7" s="20"/>
+      <c r="B7" s="17"/>
+      <c r="C7" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F7" s="5"/>
+    </row>
+    <row r="8" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="A8" s="20"/>
+      <c r="B8" s="17"/>
+      <c r="C8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F8" s="5"/>
+    </row>
+    <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.2">
+      <c r="A9" s="20"/>
+      <c r="B9" s="17"/>
+      <c r="C9" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" s="5"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="20"/>
+      <c r="B10" s="17"/>
+      <c r="C10" s="25" t="s">
+        <v>36</v>
+      </c>
+      <c r="D10" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="F10" s="27"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="20"/>
+      <c r="B11" s="17"/>
+      <c r="C11" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="D11" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="F11" s="27"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="20"/>
+      <c r="B12" s="17"/>
+      <c r="C12" s="25" t="s">
+        <v>39</v>
+      </c>
+      <c r="D12" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="E12" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="F12" s="27"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="20"/>
+      <c r="B13" s="17"/>
+      <c r="C13" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="D13" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="F13" s="27"/>
+    </row>
+    <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.2">
+      <c r="A14" s="21"/>
+      <c r="B14" s="18"/>
+      <c r="C14" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F14" s="5"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" s="19">
+        <v>3</v>
+      </c>
+      <c r="B15" s="16" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.2">
-      <c r="A4" s="6">
-        <v>2</v>
-      </c>
-      <c r="B4" s="3" t="s">
+      <c r="C15" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F15" s="5"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" s="21"/>
+      <c r="B16" s="18"/>
+      <c r="C16" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F16" s="5"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" s="19">
+        <v>4</v>
+      </c>
+      <c r="B17" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F17" s="5"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" s="20"/>
+      <c r="B18" s="17"/>
+      <c r="C18" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" s="5"/>
-    </row>
-    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.2">
-      <c r="A5" s="6">
-        <v>3</v>
-      </c>
-      <c r="B5" s="2" t="s">
+      <c r="D18" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F18" s="5"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" s="20"/>
+      <c r="B19" s="17"/>
+      <c r="C19" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F19" s="5"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" s="20"/>
+      <c r="B20" s="17"/>
+      <c r="C20" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F20" s="5"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" s="21"/>
+      <c r="B21" s="18"/>
+      <c r="C21" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" s="10">
+        <v>5</v>
+      </c>
+      <c r="B22" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="5"/>
+    </row>
+    <row r="23" spans="1:6" ht="30" x14ac:dyDescent="0.2">
+      <c r="A23" s="19">
+        <v>6</v>
+      </c>
+      <c r="B23" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F23" s="5"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24" s="20"/>
+      <c r="B24" s="23"/>
+      <c r="C24" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F24" s="5"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25" s="21"/>
+      <c r="B25" s="24"/>
+      <c r="C25" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F25" s="5"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26" s="10">
+        <v>7</v>
+      </c>
+      <c r="B26" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F26" s="5"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27" s="19">
         <v>8</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" s="3" t="s">
+      <c r="B27" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D27" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E27" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="F27" s="9"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28" s="21"/>
+      <c r="B28" s="18"/>
+      <c r="C28" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E28" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="F28" s="9"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A29" s="19">
         <v>9</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="B29" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D29" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E29" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="F29" s="9"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A30" s="21"/>
+      <c r="B30" s="18"/>
+      <c r="C30" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E30" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="F30" s="9"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A31" s="19">
         <v>10</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="6">
-        <v>4</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E6" s="5"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="6">
-        <v>5</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E7" s="5"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="6">
-        <v>6</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E8" s="5"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="10">
-        <v>7</v>
-      </c>
-      <c r="B9" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D9" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="E9" s="12" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="7">
-        <v>8</v>
-      </c>
-      <c r="B10" s="8" t="s">
+      <c r="B31" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D31" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E31" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="F31" s="9"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A32" s="20"/>
+      <c r="B32" s="17"/>
+      <c r="C32" s="28" t="s">
+        <v>27</v>
+      </c>
+      <c r="D32" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E32" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F32" s="9"/>
+    </row>
+    <row r="33" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="29"/>
+      <c r="B33" s="30"/>
+      <c r="C33" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="D10" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="E10" s="9"/>
+      <c r="D33" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E33" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F33" s="7"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="20">
+    <mergeCell ref="A31:A33"/>
+    <mergeCell ref="B31:B33"/>
+    <mergeCell ref="A23:A25"/>
+    <mergeCell ref="B23:B25"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="A29:A30"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="A6:A14"/>
+    <mergeCell ref="B6:B14"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="A17:A21"/>
+    <mergeCell ref="B17:B21"/>
     <mergeCell ref="A1:A2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:E1"/>
     <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="B3:B5"/>
+    <mergeCell ref="A3:A5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup paperSize="9" scale="96" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>